<commit_message>
Changed tree to stem
Changed tree to stem for naming consistancy. Also testing that edits and merging works
</commit_message>
<xml_diff>
--- a/testthat/table of tests 2022.xlsx
+++ b/testthat/table of tests 2022.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gmuedu-my.sharepoint.com/personal/emacmoni_gmu_edu/Documents/Documents/tree mortality cencus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gmuedu-my.sharepoint.com/personal/emacmoni_gmu_edu/Documents/Documents/GitHub/SCBImortality/testthat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D41E8AF6-9DA2-4BF1-B43A-52A668003EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{D41E8AF6-9DA2-4BF1-B43A-52A668003EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC5000A8-FF4E-4E68-9AB6-33DA5524D26D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D0E4442A-654A-47EF-988D-7FC9A44E8E29}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>warning (W) or error (E)</t>
   </si>
   <si>
-    <t>coded</t>
-  </si>
-  <si>
     <t>requires field fix?</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>use latest record</t>
   </si>
   <si>
-    <t>tree</t>
-  </si>
-  <si>
     <t>newly censused trees (A, AU, DS)</t>
   </si>
   <si>
@@ -901,6 +895,12 @@
   </si>
   <si>
     <t>not yet</t>
+  </si>
+  <si>
+    <t>stem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implimented </t>
   </si>
 </sst>
 </file>
@@ -1302,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2503491-7FCD-4D1D-8C5A-E6F72456FF07}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1313,11 +1313,12 @@
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="32.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="60">
@@ -1340,16 +1341,16 @@
         <v>7</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30">
@@ -1360,28 +1361,28 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="105">
@@ -1392,28 +1393,28 @@
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30">
@@ -1421,31 +1422,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45">
@@ -1453,31 +1454,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="J5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30">
@@ -1485,31 +1486,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="42.75">
@@ -1517,31 +1518,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="42.75">
@@ -1549,31 +1550,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="53.25">
@@ -1581,31 +1582,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="J9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30">
@@ -1613,31 +1614,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="233.25">
@@ -1645,31 +1646,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="J11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="45">
@@ -1677,31 +1678,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="J12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60">
@@ -1709,31 +1710,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45">
@@ -1741,31 +1742,31 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G14" s="4">
         <v>2021</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="186">
@@ -1773,31 +1774,31 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="60">
@@ -1805,31 +1806,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="60">
@@ -1837,31 +1838,31 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="75">
@@ -1869,31 +1870,31 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="87.75">
@@ -1901,31 +1902,31 @@
         <v>19</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="J19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="87.75">
@@ -1933,31 +1934,31 @@
         <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="J20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="75">
@@ -1965,31 +1966,31 @@
         <v>21</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="J21" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="117.75">
@@ -1997,31 +1998,31 @@
         <v>22</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="J22" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="45">
@@ -2029,31 +2030,31 @@
         <v>23</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23" s="4">
         <v>2021</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45">
@@ -2061,31 +2062,31 @@
         <v>24</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G24" s="4">
         <v>2021</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="100.5">
@@ -2093,31 +2094,31 @@
         <v>25</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="60">
@@ -2125,31 +2126,31 @@
         <v>26</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="4">
-        <v>2021</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="J26" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="60">
@@ -2157,31 +2158,31 @@
         <v>27</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G27" s="4">
         <v>2021</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="60">
@@ -2189,31 +2190,31 @@
         <v>28</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G28" s="4">
         <v>2021</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="60">
@@ -2221,31 +2222,31 @@
         <v>29</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" s="4">
         <v>2021</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="90">
@@ -2253,31 +2254,31 @@
         <v>30</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G30" s="4">
         <v>2021</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="120">
@@ -2285,31 +2286,31 @@
         <v>31</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G31" s="4">
         <v>2021</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="75">
@@ -2317,31 +2318,36 @@
         <v>32</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="I32" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>